<commit_message>
Update shiny with favicon and URLs
</commit_message>
<xml_diff>
--- a/data/example_BioPlex_plate1.xlsx
+++ b/data/example_BioPlex_plate1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wehieduau-my.sharepoint.com/personal/argyropoulos_d_wehi_edu_au/Documents/2_Projects/#PvSeroTaT/App_Shiny/PvSeroApp_Web/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/argyropoulos.d/Documents/GitHub/pvserotat/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="227" documentId="11_9D5AECD6DB7619A07CF166816CB8D5512364DE62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE855375-94C8-7040-B13A-0196FE0073AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B9F53E-BDA7-7444-8CC2-EB6F1558F22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34220" yWindow="-6160" windowWidth="22760" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45000" yWindow="-5880" windowWidth="22760" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bioplex_example" sheetId="1" r:id="rId1"/>
@@ -1112,9 +1112,6 @@
     <t>182 (120)</t>
   </si>
   <si>
-    <t>2208 (121)</t>
-  </si>
-  <si>
     <t>936 (79)</t>
   </si>
   <si>
@@ -1136,9 +1133,6 @@
     <t>58 (103)</t>
   </si>
   <si>
-    <t>712.5 (132)</t>
-  </si>
-  <si>
     <t>122 (99)</t>
   </si>
   <si>
@@ -1160,9 +1154,6 @@
     <t>221.5 (104)</t>
   </si>
   <si>
-    <t>448 (111)</t>
-  </si>
-  <si>
     <t>293 (95)</t>
   </si>
   <si>
@@ -1184,9 +1175,6 @@
     <t>48 (135)</t>
   </si>
   <si>
-    <t>480 (132)</t>
-  </si>
-  <si>
     <t>109 (79)</t>
   </si>
   <si>
@@ -1208,9 +1196,6 @@
     <t>209.5 (110)</t>
   </si>
   <si>
-    <t>650 (137)</t>
-  </si>
-  <si>
     <t>1665.5 (86)</t>
   </si>
   <si>
@@ -1232,9 +1217,6 @@
     <t>70 (128)</t>
   </si>
   <si>
-    <t>293.5 (110)</t>
-  </si>
-  <si>
     <t>294.5 (84)</t>
   </si>
   <si>
@@ -1256,9 +1238,6 @@
     <t>962 (101)</t>
   </si>
   <si>
-    <t>1632.5 (126)</t>
-  </si>
-  <si>
     <t>241 (78)</t>
   </si>
   <si>
@@ -1328,9 +1307,6 @@
     <t>2342 (118)</t>
   </si>
   <si>
-    <t>9995.5 (168)</t>
-  </si>
-  <si>
     <t>1992 (77)</t>
   </si>
   <si>
@@ -1352,9 +1328,6 @@
     <t>535.5 (90)</t>
   </si>
   <si>
-    <t>12560 (112)</t>
-  </si>
-  <si>
     <t>8821 (85)</t>
   </si>
   <si>
@@ -1376,9 +1349,6 @@
     <t>306 (109)</t>
   </si>
   <si>
-    <t>2060 (125)</t>
-  </si>
-  <si>
     <t>315 (88)</t>
   </si>
   <si>
@@ -1400,9 +1370,6 @@
     <t>100 (93)</t>
   </si>
   <si>
-    <t>443 (132)</t>
-  </si>
-  <si>
     <t>652 (81)</t>
   </si>
   <si>
@@ -1424,9 +1391,6 @@
     <t>79 (107)</t>
   </si>
   <si>
-    <t>3212 (149)</t>
-  </si>
-  <si>
     <t>179 (90)</t>
   </si>
   <si>
@@ -1448,9 +1412,6 @@
     <t>390 (105)</t>
   </si>
   <si>
-    <t>15769.5 (150)</t>
-  </si>
-  <si>
     <t>8814 (87)</t>
   </si>
   <si>
@@ -1472,9 +1433,6 @@
     <t>1777.5 (112)</t>
   </si>
   <si>
-    <t>6845 (131)</t>
-  </si>
-  <si>
     <t>2465 (91)</t>
   </si>
   <si>
@@ -1520,9 +1478,6 @@
     <t>3017 (97)</t>
   </si>
   <si>
-    <t>5339 (123)</t>
-  </si>
-  <si>
     <t>4928 (87)</t>
   </si>
   <si>
@@ -1544,9 +1499,6 @@
     <t>2575.5 (130)</t>
   </si>
   <si>
-    <t>4592.5 (144)</t>
-  </si>
-  <si>
     <t>2779 (95)</t>
   </si>
   <si>
@@ -1568,9 +1520,6 @@
     <t>9860 (89)</t>
   </si>
   <si>
-    <t>19340.5 (114)</t>
-  </si>
-  <si>
     <t>5612 (77)</t>
   </si>
   <si>
@@ -1640,9 +1589,6 @@
     <t>3973 (97)</t>
   </si>
   <si>
-    <t>2812 (128)</t>
-  </si>
-  <si>
     <t>803 (62)</t>
   </si>
   <si>
@@ -1664,9 +1610,6 @@
     <t>11482.5 (98)</t>
   </si>
   <si>
-    <t>17816 (121)</t>
-  </si>
-  <si>
     <t>4830.5 (80)</t>
   </si>
   <si>
@@ -1688,9 +1631,6 @@
     <t>168 (90)</t>
   </si>
   <si>
-    <t>315 (127)</t>
-  </si>
-  <si>
     <t>908 (83)</t>
   </si>
   <si>
@@ -1736,9 +1676,6 @@
     <t>986 (103)</t>
   </si>
   <si>
-    <t>1562 (145)</t>
-  </si>
-  <si>
     <t>299.5 (84)</t>
   </si>
   <si>
@@ -1760,9 +1697,6 @@
     <t>89 (116)</t>
   </si>
   <si>
-    <t>893.5 (134)</t>
-  </si>
-  <si>
     <t>410 (77)</t>
   </si>
   <si>
@@ -1784,9 +1718,6 @@
     <t>66 (109)</t>
   </si>
   <si>
-    <t>418.5 (124)</t>
-  </si>
-  <si>
     <t>200 (94)</t>
   </si>
   <si>
@@ -1808,9 +1739,6 @@
     <t>137 (118)</t>
   </si>
   <si>
-    <t>13029.5 (138)</t>
-  </si>
-  <si>
     <t>1762 (81)</t>
   </si>
   <si>
@@ -1832,9 +1760,6 @@
     <t>78 (89)</t>
   </si>
   <si>
-    <t>4540 (125)</t>
-  </si>
-  <si>
     <t>1513.5 (72)</t>
   </si>
   <si>
@@ -1880,9 +1805,6 @@
     <t>791 (101)</t>
   </si>
   <si>
-    <t>2621 (130)</t>
-  </si>
-  <si>
     <t>417.5 (64)</t>
   </si>
   <si>
@@ -1904,9 +1826,6 @@
     <t>1479.5 (108)</t>
   </si>
   <si>
-    <t>2637.5 (134)</t>
-  </si>
-  <si>
     <t>1504 (81)</t>
   </si>
   <si>
@@ -1928,9 +1847,6 @@
     <t>48 (84)</t>
   </si>
   <si>
-    <t>570 (119)</t>
-  </si>
-  <si>
     <t>183 (69)</t>
   </si>
   <si>
@@ -1952,9 +1868,6 @@
     <t>204.5 (100)</t>
   </si>
   <si>
-    <t>8897 (147)</t>
-  </si>
-  <si>
     <t>504 (81)</t>
   </si>
   <si>
@@ -2000,9 +1913,6 @@
     <t>141 (85)</t>
   </si>
   <si>
-    <t>15119.5 (144)</t>
-  </si>
-  <si>
     <t>2147 (88)</t>
   </si>
   <si>
@@ -2024,9 +1934,6 @@
     <t>90 (125)</t>
   </si>
   <si>
-    <t>4799 (141)</t>
-  </si>
-  <si>
     <t>2178 (91)</t>
   </si>
   <si>
@@ -2048,9 +1955,6 @@
     <t>142.5 (96)</t>
   </si>
   <si>
-    <t>323.5 (164)</t>
-  </si>
-  <si>
     <t>298 (51)</t>
   </si>
   <si>
@@ -2072,9 +1976,6 @@
     <t>507 (109)</t>
   </si>
   <si>
-    <t>3584 (118)</t>
-  </si>
-  <si>
     <t>709 (86)</t>
   </si>
   <si>
@@ -2120,9 +2021,6 @@
     <t>4833 (101)</t>
   </si>
   <si>
-    <t>16718 (147)</t>
-  </si>
-  <si>
     <t>5329 (72)</t>
   </si>
   <si>
@@ -2144,9 +2042,6 @@
     <t>7426 (117)</t>
   </si>
   <si>
-    <t>14663 (125)</t>
-  </si>
-  <si>
     <t>4826 (75)</t>
   </si>
   <si>
@@ -2168,9 +2063,6 @@
     <t>535.5 (98)</t>
   </si>
   <si>
-    <t>21105 (115)</t>
-  </si>
-  <si>
     <t>7928.5 (90)</t>
   </si>
   <si>
@@ -2192,9 +2084,6 @@
     <t>9357 (114)</t>
   </si>
   <si>
-    <t>11769.5 (128)</t>
-  </si>
-  <si>
     <t>3736 (73)</t>
   </si>
   <si>
@@ -2237,9 +2126,6 @@
     <t>586 (161)</t>
   </si>
   <si>
-    <t>5129 (125)</t>
-  </si>
-  <si>
     <t>425.5 (64)</t>
   </si>
   <si>
@@ -2261,9 +2147,6 @@
     <t>1289 (94)</t>
   </si>
   <si>
-    <t>24039.5 (120)</t>
-  </si>
-  <si>
     <t>13891 (85)</t>
   </si>
   <si>
@@ -2285,9 +2168,6 @@
     <t>12307 (100)</t>
   </si>
   <si>
-    <t>14907 (119)</t>
-  </si>
-  <si>
     <t>4157 (66)</t>
   </si>
   <si>
@@ -2405,9 +2285,6 @@
     <t>59 (101)</t>
   </si>
   <si>
-    <t>2999 (124)</t>
-  </si>
-  <si>
     <t>655 (80)</t>
   </si>
   <si>
@@ -2429,9 +2306,6 @@
     <t>55 (118)</t>
   </si>
   <si>
-    <t>491 (156)</t>
-  </si>
-  <si>
     <t>681.5 (70)</t>
   </si>
   <si>
@@ -2453,9 +2327,6 @@
     <t>9692 (101)</t>
   </si>
   <si>
-    <t>10115 (126)</t>
-  </si>
-  <si>
     <t>9513 (85)</t>
   </si>
   <si>
@@ -2525,9 +2396,6 @@
     <t>7436 (98)</t>
   </si>
   <si>
-    <t>8361 (113)</t>
-  </si>
-  <si>
     <t>4111.5 (86)</t>
   </si>
   <si>
@@ -2573,9 +2441,6 @@
     <t>79 (90)</t>
   </si>
   <si>
-    <t>7995 (119)</t>
-  </si>
-  <si>
     <t>2080 (73)</t>
   </si>
   <si>
@@ -2597,9 +2462,6 @@
     <t>167.5 (106)</t>
   </si>
   <si>
-    <t>5080.5 (164)</t>
-  </si>
-  <si>
     <t>1553 (79)</t>
   </si>
   <si>
@@ -2621,9 +2483,6 @@
     <t>181 (102)</t>
   </si>
   <si>
-    <t>13904.5 (106)</t>
-  </si>
-  <si>
     <t>1660.5 (82)</t>
   </si>
   <si>
@@ -2645,9 +2504,6 @@
     <t>278 (91)</t>
   </si>
   <si>
-    <t>17653 (111)</t>
-  </si>
-  <si>
     <t>2052.5 (80)</t>
   </si>
   <si>
@@ -2693,9 +2549,6 @@
     <t>2247.5 (74)</t>
   </si>
   <si>
-    <t>4179 (138)</t>
-  </si>
-  <si>
     <t>590 (70)</t>
   </si>
   <si>
@@ -2741,9 +2594,6 @@
     <t>95 (100)</t>
   </si>
   <si>
-    <t>1303 (111)</t>
-  </si>
-  <si>
     <t>396 (53)</t>
   </si>
   <si>
@@ -2765,9 +2615,6 @@
     <t>135.5 (78)</t>
   </si>
   <si>
-    <t>5677 (108)</t>
-  </si>
-  <si>
     <t>292 (59)</t>
   </si>
   <si>
@@ -2813,9 +2660,6 @@
     <t>68 (95)</t>
   </si>
   <si>
-    <t>9563 (111)</t>
-  </si>
-  <si>
     <t>960 (73)</t>
   </si>
   <si>
@@ -2834,9 +2678,6 @@
     <t>66 (129)</t>
   </si>
   <si>
-    <t>2006 (140)</t>
-  </si>
-  <si>
     <t>1724.5 (96)</t>
   </si>
   <si>
@@ -2882,9 +2723,6 @@
     <t>469.5 (94)</t>
   </si>
   <si>
-    <t>2230.5 (122)</t>
-  </si>
-  <si>
     <t>345 (62)</t>
   </si>
   <si>
@@ -2930,9 +2768,6 @@
     <t>2319.5 (108)</t>
   </si>
   <si>
-    <t>7904.5 (100)</t>
-  </si>
-  <si>
     <t>1521 (56)</t>
   </si>
   <si>
@@ -2978,9 +2813,6 @@
     <t>325 (96)</t>
   </si>
   <si>
-    <t>16791 (97)</t>
-  </si>
-  <si>
     <t>4608 (71)</t>
   </si>
   <si>
@@ -3002,9 +2834,6 @@
     <t>6106 (109)</t>
   </si>
   <si>
-    <t>7444 (131)</t>
-  </si>
-  <si>
     <t>1303 (83)</t>
   </si>
   <si>
@@ -3047,9 +2876,6 @@
     <t>66 (81)</t>
   </si>
   <si>
-    <t>3743 (124)</t>
-  </si>
-  <si>
     <t>261 (62)</t>
   </si>
   <si>
@@ -3071,9 +2897,6 @@
     <t>645 (72)</t>
   </si>
   <si>
-    <t>18881 (86)</t>
-  </si>
-  <si>
     <t>8856 (74)</t>
   </si>
   <si>
@@ -3095,13 +2918,190 @@
     <t>7423 (81)</t>
   </si>
   <si>
-    <t>9494 (127)</t>
-  </si>
-  <si>
     <t>1841.5 (76)</t>
   </si>
   <si>
     <t>335 (83)</t>
+  </si>
+  <si>
+    <t>1068 (121)</t>
+  </si>
+  <si>
+    <t>465.5 (132)</t>
+  </si>
+  <si>
+    <t>463 (111)</t>
+  </si>
+  <si>
+    <t>591 (132)</t>
+  </si>
+  <si>
+    <t>671 (137)</t>
+  </si>
+  <si>
+    <t>103 (110)</t>
+  </si>
+  <si>
+    <t>1441.5 (126)</t>
+  </si>
+  <si>
+    <t>1386 (168)</t>
+  </si>
+  <si>
+    <t>1575 (112)</t>
+  </si>
+  <si>
+    <t>590 (125)</t>
+  </si>
+  <si>
+    <t>301 (132)</t>
+  </si>
+  <si>
+    <t>1090 (149)</t>
+  </si>
+  <si>
+    <t>6704 (150)</t>
+  </si>
+  <si>
+    <t>2390 (131)</t>
+  </si>
+  <si>
+    <t>1034 (123)</t>
+  </si>
+  <si>
+    <t>2903 (144)</t>
+  </si>
+  <si>
+    <t>13703 (114)</t>
+  </si>
+  <si>
+    <t>1426.5 (128)</t>
+  </si>
+  <si>
+    <t>12031 (121)</t>
+  </si>
+  <si>
+    <t>488 (127)</t>
+  </si>
+  <si>
+    <t>1041 (145)</t>
+  </si>
+  <si>
+    <t>203 (134)</t>
+  </si>
+  <si>
+    <t>205 (124)</t>
+  </si>
+  <si>
+    <t>2032 (138)</t>
+  </si>
+  <si>
+    <t>903 (125)</t>
+  </si>
+  <si>
+    <t>1093 (130)</t>
+  </si>
+  <si>
+    <t>899 (134)</t>
+  </si>
+  <si>
+    <t>400 (119)</t>
+  </si>
+  <si>
+    <t>1090 (147)</t>
+  </si>
+  <si>
+    <t>1993 (144)</t>
+  </si>
+  <si>
+    <t>600 (141)</t>
+  </si>
+  <si>
+    <t>280 (164)</t>
+  </si>
+  <si>
+    <t>1009 (118)</t>
+  </si>
+  <si>
+    <t>2340 (147)</t>
+  </si>
+  <si>
+    <t>11930 (125)</t>
+  </si>
+  <si>
+    <t>14032 (115)</t>
+  </si>
+  <si>
+    <t>8009 (128)</t>
+  </si>
+  <si>
+    <t>830 (125)</t>
+  </si>
+  <si>
+    <t>12930 (120)</t>
+  </si>
+  <si>
+    <t>5029 (119)</t>
+  </si>
+  <si>
+    <t>480 (124)</t>
+  </si>
+  <si>
+    <t>307 (156)</t>
+  </si>
+  <si>
+    <t>8090 (126)</t>
+  </si>
+  <si>
+    <t>7361 (113)</t>
+  </si>
+  <si>
+    <t>339 (119)</t>
+  </si>
+  <si>
+    <t>1013 (164)</t>
+  </si>
+  <si>
+    <t>6160 (106)</t>
+  </si>
+  <si>
+    <t>787 (111)</t>
+  </si>
+  <si>
+    <t>3322 (138)</t>
+  </si>
+  <si>
+    <t>712 (111)</t>
+  </si>
+  <si>
+    <t>392 (108)</t>
+  </si>
+  <si>
+    <t>1020 (111)</t>
+  </si>
+  <si>
+    <t>1449 (140)</t>
+  </si>
+  <si>
+    <t>802 (122)</t>
+  </si>
+  <si>
+    <t>2009 (100)</t>
+  </si>
+  <si>
+    <t>3021 (97)</t>
+  </si>
+  <si>
+    <t>2093 (131)</t>
+  </si>
+  <si>
+    <t>990 (124)</t>
+  </si>
+  <si>
+    <t>7092 (86)</t>
+  </si>
+  <si>
+    <t>1203 (127)</t>
   </si>
 </sst>
 </file>
@@ -3437,7 +3437,7 @@
   <dimension ref="A1:O104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4121,13 +4121,13 @@
         <v>357</v>
       </c>
       <c r="H21" t="s">
+        <v>962</v>
+      </c>
+      <c r="I21" t="s">
         <v>358</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>359</v>
-      </c>
-      <c r="J21" t="s">
-        <v>360</v>
       </c>
       <c r="K21" t="s">
         <v>41</v>
@@ -4153,28 +4153,28 @@
         <v>174</v>
       </c>
       <c r="C22" t="s">
+        <v>360</v>
+      </c>
+      <c r="D22" t="s">
         <v>361</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>362</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>363</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>364</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
+        <v>963</v>
+      </c>
+      <c r="I22" t="s">
         <v>365</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>366</v>
-      </c>
-      <c r="I22" t="s">
-        <v>367</v>
-      </c>
-      <c r="J22" t="s">
-        <v>368</v>
       </c>
       <c r="K22" t="s">
         <v>43</v>
@@ -4200,28 +4200,28 @@
         <v>177</v>
       </c>
       <c r="C23" t="s">
+        <v>367</v>
+      </c>
+      <c r="D23" t="s">
+        <v>368</v>
+      </c>
+      <c r="E23" t="s">
         <v>369</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>370</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>371</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
+        <v>964</v>
+      </c>
+      <c r="I23" t="s">
         <v>372</v>
       </c>
-      <c r="G23" t="s">
+      <c r="J23" t="s">
         <v>373</v>
-      </c>
-      <c r="H23" t="s">
-        <v>374</v>
-      </c>
-      <c r="I23" t="s">
-        <v>375</v>
-      </c>
-      <c r="J23" t="s">
-        <v>376</v>
       </c>
       <c r="K23" t="s">
         <v>45</v>
@@ -4247,28 +4247,28 @@
         <v>180</v>
       </c>
       <c r="C24" t="s">
+        <v>374</v>
+      </c>
+      <c r="D24" t="s">
+        <v>375</v>
+      </c>
+      <c r="E24" t="s">
+        <v>376</v>
+      </c>
+      <c r="F24" t="s">
         <v>377</v>
       </c>
-      <c r="D24" t="s">
+      <c r="G24" t="s">
         <v>378</v>
       </c>
-      <c r="E24" t="s">
+      <c r="H24" t="s">
+        <v>965</v>
+      </c>
+      <c r="I24" t="s">
         <v>379</v>
       </c>
-      <c r="F24" t="s">
+      <c r="J24" t="s">
         <v>380</v>
-      </c>
-      <c r="G24" t="s">
-        <v>381</v>
-      </c>
-      <c r="H24" t="s">
-        <v>382</v>
-      </c>
-      <c r="I24" t="s">
-        <v>383</v>
-      </c>
-      <c r="J24" t="s">
-        <v>384</v>
       </c>
       <c r="K24" t="s">
         <v>47</v>
@@ -4294,28 +4294,28 @@
         <v>183</v>
       </c>
       <c r="C25" t="s">
+        <v>381</v>
+      </c>
+      <c r="D25" t="s">
+        <v>382</v>
+      </c>
+      <c r="E25" t="s">
+        <v>383</v>
+      </c>
+      <c r="F25" t="s">
+        <v>384</v>
+      </c>
+      <c r="G25" t="s">
         <v>385</v>
       </c>
-      <c r="D25" t="s">
+      <c r="H25" t="s">
+        <v>966</v>
+      </c>
+      <c r="I25" t="s">
         <v>386</v>
       </c>
-      <c r="E25" t="s">
+      <c r="J25" t="s">
         <v>387</v>
-      </c>
-      <c r="F25" t="s">
-        <v>388</v>
-      </c>
-      <c r="G25" t="s">
-        <v>389</v>
-      </c>
-      <c r="H25" t="s">
-        <v>390</v>
-      </c>
-      <c r="I25" t="s">
-        <v>391</v>
-      </c>
-      <c r="J25" t="s">
-        <v>392</v>
       </c>
       <c r="K25" t="s">
         <v>50</v>
@@ -4341,28 +4341,28 @@
         <v>186</v>
       </c>
       <c r="C26" t="s">
+        <v>388</v>
+      </c>
+      <c r="D26" t="s">
+        <v>389</v>
+      </c>
+      <c r="E26" t="s">
+        <v>390</v>
+      </c>
+      <c r="F26" t="s">
+        <v>391</v>
+      </c>
+      <c r="G26" t="s">
+        <v>392</v>
+      </c>
+      <c r="H26" t="s">
+        <v>967</v>
+      </c>
+      <c r="I26" t="s">
         <v>393</v>
       </c>
-      <c r="D26" t="s">
+      <c r="J26" t="s">
         <v>394</v>
-      </c>
-      <c r="E26" t="s">
-        <v>395</v>
-      </c>
-      <c r="F26" t="s">
-        <v>396</v>
-      </c>
-      <c r="G26" t="s">
-        <v>397</v>
-      </c>
-      <c r="H26" t="s">
-        <v>398</v>
-      </c>
-      <c r="I26" t="s">
-        <v>399</v>
-      </c>
-      <c r="J26" t="s">
-        <v>400</v>
       </c>
       <c r="K26" t="s">
         <v>52</v>
@@ -4388,28 +4388,28 @@
         <v>189</v>
       </c>
       <c r="C27" t="s">
+        <v>395</v>
+      </c>
+      <c r="D27" t="s">
+        <v>396</v>
+      </c>
+      <c r="E27" t="s">
+        <v>397</v>
+      </c>
+      <c r="F27" t="s">
+        <v>398</v>
+      </c>
+      <c r="G27" t="s">
+        <v>399</v>
+      </c>
+      <c r="H27" t="s">
+        <v>968</v>
+      </c>
+      <c r="I27" t="s">
+        <v>400</v>
+      </c>
+      <c r="J27" t="s">
         <v>401</v>
-      </c>
-      <c r="D27" t="s">
-        <v>402</v>
-      </c>
-      <c r="E27" t="s">
-        <v>403</v>
-      </c>
-      <c r="F27" t="s">
-        <v>404</v>
-      </c>
-      <c r="G27" t="s">
-        <v>405</v>
-      </c>
-      <c r="H27" t="s">
-        <v>406</v>
-      </c>
-      <c r="I27" t="s">
-        <v>407</v>
-      </c>
-      <c r="J27" t="s">
-        <v>408</v>
       </c>
       <c r="K27" t="s">
         <v>54</v>
@@ -4435,28 +4435,28 @@
         <v>192</v>
       </c>
       <c r="C28" t="s">
+        <v>402</v>
+      </c>
+      <c r="D28" t="s">
+        <v>403</v>
+      </c>
+      <c r="E28" t="s">
+        <v>404</v>
+      </c>
+      <c r="F28" t="s">
+        <v>405</v>
+      </c>
+      <c r="G28" t="s">
+        <v>406</v>
+      </c>
+      <c r="H28" t="s">
+        <v>407</v>
+      </c>
+      <c r="I28" t="s">
+        <v>408</v>
+      </c>
+      <c r="J28" t="s">
         <v>409</v>
-      </c>
-      <c r="D28" t="s">
-        <v>410</v>
-      </c>
-      <c r="E28" t="s">
-        <v>411</v>
-      </c>
-      <c r="F28" t="s">
-        <v>412</v>
-      </c>
-      <c r="G28" t="s">
-        <v>413</v>
-      </c>
-      <c r="H28" t="s">
-        <v>414</v>
-      </c>
-      <c r="I28" t="s">
-        <v>415</v>
-      </c>
-      <c r="J28" t="s">
-        <v>416</v>
       </c>
       <c r="K28" t="s">
         <v>16</v>
@@ -4482,28 +4482,28 @@
         <v>195</v>
       </c>
       <c r="C29" t="s">
+        <v>410</v>
+      </c>
+      <c r="D29" t="s">
+        <v>411</v>
+      </c>
+      <c r="E29" t="s">
+        <v>412</v>
+      </c>
+      <c r="F29" t="s">
+        <v>413</v>
+      </c>
+      <c r="G29" t="s">
+        <v>414</v>
+      </c>
+      <c r="H29" t="s">
+        <v>415</v>
+      </c>
+      <c r="I29" t="s">
+        <v>416</v>
+      </c>
+      <c r="J29" t="s">
         <v>417</v>
-      </c>
-      <c r="D29" t="s">
-        <v>418</v>
-      </c>
-      <c r="E29" t="s">
-        <v>419</v>
-      </c>
-      <c r="F29" t="s">
-        <v>420</v>
-      </c>
-      <c r="G29" t="s">
-        <v>421</v>
-      </c>
-      <c r="H29" t="s">
-        <v>422</v>
-      </c>
-      <c r="I29" t="s">
-        <v>423</v>
-      </c>
-      <c r="J29" t="s">
-        <v>424</v>
       </c>
       <c r="K29" t="s">
         <v>58</v>
@@ -4529,28 +4529,28 @@
         <v>200</v>
       </c>
       <c r="C30" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="D30" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="E30" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="F30" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="G30" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="H30" t="s">
-        <v>430</v>
+        <v>969</v>
       </c>
       <c r="I30" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="J30" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="K30" t="s">
         <v>60</v>
@@ -4576,28 +4576,28 @@
         <v>203</v>
       </c>
       <c r="C31" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="D31" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="E31" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="F31" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="G31" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="H31" t="s">
-        <v>438</v>
+        <v>970</v>
       </c>
       <c r="I31" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
       <c r="J31" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
       <c r="K31" t="s">
         <v>62</v>
@@ -4623,28 +4623,28 @@
         <v>172</v>
       </c>
       <c r="C32" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
       <c r="D32" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="E32" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="F32" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="G32" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="H32" t="s">
-        <v>446</v>
+        <v>971</v>
       </c>
       <c r="I32" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="J32" t="s">
-        <v>448</v>
+        <v>438</v>
       </c>
       <c r="K32" t="s">
         <v>64</v>
@@ -4670,28 +4670,28 @@
         <v>175</v>
       </c>
       <c r="C33" t="s">
-        <v>449</v>
+        <v>439</v>
       </c>
       <c r="D33" t="s">
-        <v>450</v>
+        <v>440</v>
       </c>
       <c r="E33" t="s">
-        <v>451</v>
+        <v>441</v>
       </c>
       <c r="F33" t="s">
-        <v>452</v>
+        <v>442</v>
       </c>
       <c r="G33" t="s">
-        <v>453</v>
+        <v>443</v>
       </c>
       <c r="H33" t="s">
-        <v>454</v>
+        <v>972</v>
       </c>
       <c r="I33" t="s">
-        <v>455</v>
+        <v>444</v>
       </c>
       <c r="J33" t="s">
-        <v>456</v>
+        <v>445</v>
       </c>
       <c r="K33" t="s">
         <v>67</v>
@@ -4717,28 +4717,28 @@
         <v>178</v>
       </c>
       <c r="C34" t="s">
-        <v>457</v>
+        <v>446</v>
       </c>
       <c r="D34" t="s">
-        <v>458</v>
+        <v>447</v>
       </c>
       <c r="E34" t="s">
-        <v>459</v>
+        <v>448</v>
       </c>
       <c r="F34" t="s">
-        <v>460</v>
+        <v>449</v>
       </c>
       <c r="G34" t="s">
-        <v>461</v>
+        <v>450</v>
       </c>
       <c r="H34" t="s">
-        <v>462</v>
+        <v>973</v>
       </c>
       <c r="I34" t="s">
-        <v>463</v>
+        <v>451</v>
       </c>
       <c r="J34" t="s">
-        <v>464</v>
+        <v>452</v>
       </c>
       <c r="K34" t="s">
         <v>69</v>
@@ -4764,28 +4764,28 @@
         <v>181</v>
       </c>
       <c r="C35" t="s">
-        <v>465</v>
+        <v>453</v>
       </c>
       <c r="D35" t="s">
-        <v>466</v>
+        <v>454</v>
       </c>
       <c r="E35" t="s">
-        <v>467</v>
+        <v>455</v>
       </c>
       <c r="F35" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="G35" t="s">
-        <v>469</v>
+        <v>457</v>
       </c>
       <c r="H35" t="s">
-        <v>470</v>
+        <v>974</v>
       </c>
       <c r="I35" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="J35" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="K35" t="s">
         <v>71</v>
@@ -4811,28 +4811,28 @@
         <v>184</v>
       </c>
       <c r="C36" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="D36" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="E36" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
       <c r="F36" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="G36" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="H36" t="s">
-        <v>478</v>
+        <v>975</v>
       </c>
       <c r="I36" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="J36" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="K36" t="s">
         <v>29</v>
@@ -4858,28 +4858,28 @@
         <v>187</v>
       </c>
       <c r="C37" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="D37" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="E37" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="F37" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="G37" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="H37" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="I37" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="J37" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="K37" t="s">
         <v>75</v>
@@ -4905,28 +4905,28 @@
         <v>190</v>
       </c>
       <c r="C38" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="D38" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="E38" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="F38" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="G38" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="H38" t="s">
-        <v>494</v>
+        <v>976</v>
       </c>
       <c r="I38" t="s">
-        <v>495</v>
+        <v>480</v>
       </c>
       <c r="J38" t="s">
-        <v>496</v>
+        <v>481</v>
       </c>
       <c r="K38" t="s">
         <v>77</v>
@@ -4952,28 +4952,28 @@
         <v>193</v>
       </c>
       <c r="C39" t="s">
-        <v>497</v>
+        <v>482</v>
       </c>
       <c r="D39" t="s">
-        <v>498</v>
+        <v>483</v>
       </c>
       <c r="E39" t="s">
-        <v>499</v>
+        <v>484</v>
       </c>
       <c r="F39" t="s">
-        <v>500</v>
+        <v>485</v>
       </c>
       <c r="G39" t="s">
-        <v>501</v>
+        <v>486</v>
       </c>
       <c r="H39" t="s">
-        <v>502</v>
+        <v>977</v>
       </c>
       <c r="I39" t="s">
-        <v>503</v>
+        <v>487</v>
       </c>
       <c r="J39" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="K39" t="s">
         <v>79</v>
@@ -4999,28 +4999,28 @@
         <v>196</v>
       </c>
       <c r="C40" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
       <c r="D40" t="s">
-        <v>506</v>
+        <v>490</v>
       </c>
       <c r="E40" t="s">
-        <v>507</v>
+        <v>491</v>
       </c>
       <c r="F40" t="s">
-        <v>508</v>
+        <v>492</v>
       </c>
       <c r="G40" t="s">
-        <v>509</v>
+        <v>493</v>
       </c>
       <c r="H40" t="s">
-        <v>510</v>
+        <v>978</v>
       </c>
       <c r="I40" t="s">
-        <v>511</v>
+        <v>494</v>
       </c>
       <c r="J40" t="s">
-        <v>512</v>
+        <v>495</v>
       </c>
       <c r="K40" t="s">
         <v>81</v>
@@ -5046,28 +5046,28 @@
         <v>198</v>
       </c>
       <c r="C41" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="D41" t="s">
-        <v>514</v>
+        <v>497</v>
       </c>
       <c r="E41" t="s">
-        <v>515</v>
+        <v>498</v>
       </c>
       <c r="F41" t="s">
-        <v>516</v>
+        <v>499</v>
       </c>
       <c r="G41" t="s">
-        <v>517</v>
+        <v>500</v>
       </c>
       <c r="H41" t="s">
-        <v>518</v>
+        <v>501</v>
       </c>
       <c r="I41" t="s">
-        <v>519</v>
+        <v>502</v>
       </c>
       <c r="J41" t="s">
-        <v>520</v>
+        <v>503</v>
       </c>
       <c r="K41" t="s">
         <v>84</v>
@@ -5093,28 +5093,28 @@
         <v>201</v>
       </c>
       <c r="C42" t="s">
-        <v>521</v>
+        <v>504</v>
       </c>
       <c r="D42" t="s">
-        <v>522</v>
+        <v>505</v>
       </c>
       <c r="E42" t="s">
-        <v>523</v>
+        <v>506</v>
       </c>
       <c r="F42" t="s">
-        <v>524</v>
+        <v>507</v>
       </c>
       <c r="G42" t="s">
-        <v>525</v>
+        <v>508</v>
       </c>
       <c r="H42" t="s">
-        <v>526</v>
+        <v>509</v>
       </c>
       <c r="I42" t="s">
-        <v>527</v>
+        <v>510</v>
       </c>
       <c r="J42" t="s">
-        <v>528</v>
+        <v>511</v>
       </c>
       <c r="K42" t="s">
         <v>86</v>
@@ -5140,28 +5140,28 @@
         <v>204</v>
       </c>
       <c r="C43" t="s">
-        <v>529</v>
+        <v>512</v>
       </c>
       <c r="D43" t="s">
-        <v>530</v>
+        <v>513</v>
       </c>
       <c r="E43" t="s">
-        <v>531</v>
+        <v>514</v>
       </c>
       <c r="F43" t="s">
-        <v>532</v>
+        <v>515</v>
       </c>
       <c r="G43" t="s">
-        <v>533</v>
+        <v>516</v>
       </c>
       <c r="H43" t="s">
-        <v>534</v>
+        <v>979</v>
       </c>
       <c r="I43" t="s">
-        <v>535</v>
+        <v>517</v>
       </c>
       <c r="J43" t="s">
-        <v>536</v>
+        <v>518</v>
       </c>
       <c r="K43" t="s">
         <v>88</v>
@@ -5187,28 +5187,28 @@
         <v>173</v>
       </c>
       <c r="C44" t="s">
-        <v>537</v>
+        <v>519</v>
       </c>
       <c r="D44" t="s">
-        <v>538</v>
+        <v>520</v>
       </c>
       <c r="E44" t="s">
-        <v>539</v>
+        <v>521</v>
       </c>
       <c r="F44" t="s">
-        <v>540</v>
+        <v>522</v>
       </c>
       <c r="G44" t="s">
-        <v>541</v>
+        <v>523</v>
       </c>
       <c r="H44" t="s">
-        <v>542</v>
+        <v>980</v>
       </c>
       <c r="I44" t="s">
-        <v>543</v>
+        <v>524</v>
       </c>
       <c r="J44" t="s">
-        <v>544</v>
+        <v>525</v>
       </c>
       <c r="K44" t="s">
         <v>81</v>
@@ -5234,28 +5234,28 @@
         <v>176</v>
       </c>
       <c r="C45" t="s">
-        <v>545</v>
+        <v>526</v>
       </c>
       <c r="D45" t="s">
-        <v>546</v>
+        <v>527</v>
       </c>
       <c r="E45" t="s">
-        <v>547</v>
+        <v>528</v>
       </c>
       <c r="F45" t="s">
-        <v>548</v>
+        <v>529</v>
       </c>
       <c r="G45" t="s">
-        <v>549</v>
+        <v>530</v>
       </c>
       <c r="H45" t="s">
-        <v>550</v>
+        <v>981</v>
       </c>
       <c r="I45" t="s">
-        <v>551</v>
+        <v>531</v>
       </c>
       <c r="J45" t="s">
-        <v>552</v>
+        <v>532</v>
       </c>
       <c r="K45" t="s">
         <v>92</v>
@@ -5281,28 +5281,28 @@
         <v>179</v>
       </c>
       <c r="C46" t="s">
-        <v>553</v>
+        <v>533</v>
       </c>
       <c r="D46" t="s">
-        <v>554</v>
+        <v>534</v>
       </c>
       <c r="E46" t="s">
-        <v>555</v>
+        <v>535</v>
       </c>
       <c r="F46" t="s">
-        <v>556</v>
+        <v>536</v>
       </c>
       <c r="G46" t="s">
-        <v>557</v>
+        <v>537</v>
       </c>
       <c r="H46" t="s">
-        <v>558</v>
+        <v>538</v>
       </c>
       <c r="I46" t="s">
-        <v>559</v>
+        <v>539</v>
       </c>
       <c r="J46" t="s">
-        <v>560</v>
+        <v>540</v>
       </c>
       <c r="K46" t="s">
         <v>94</v>
@@ -5328,28 +5328,28 @@
         <v>182</v>
       </c>
       <c r="C47" t="s">
-        <v>561</v>
+        <v>541</v>
       </c>
       <c r="D47" t="s">
-        <v>562</v>
+        <v>542</v>
       </c>
       <c r="E47" t="s">
-        <v>563</v>
+        <v>543</v>
       </c>
       <c r="F47" t="s">
-        <v>564</v>
+        <v>544</v>
       </c>
       <c r="G47" t="s">
-        <v>565</v>
+        <v>545</v>
       </c>
       <c r="H47" t="s">
-        <v>566</v>
+        <v>982</v>
       </c>
       <c r="I47" t="s">
-        <v>567</v>
+        <v>546</v>
       </c>
       <c r="J47" t="s">
-        <v>568</v>
+        <v>547</v>
       </c>
       <c r="K47" t="s">
         <v>47</v>
@@ -5375,28 +5375,28 @@
         <v>185</v>
       </c>
       <c r="C48" t="s">
-        <v>569</v>
+        <v>548</v>
       </c>
       <c r="D48" t="s">
-        <v>570</v>
+        <v>549</v>
       </c>
       <c r="E48" t="s">
-        <v>571</v>
+        <v>550</v>
       </c>
       <c r="F48" t="s">
-        <v>572</v>
+        <v>551</v>
       </c>
       <c r="G48" t="s">
-        <v>573</v>
+        <v>552</v>
       </c>
       <c r="H48" t="s">
-        <v>574</v>
+        <v>983</v>
       </c>
       <c r="I48" t="s">
-        <v>575</v>
+        <v>553</v>
       </c>
       <c r="J48" t="s">
-        <v>576</v>
+        <v>554</v>
       </c>
       <c r="K48" t="s">
         <v>97</v>
@@ -5422,28 +5422,28 @@
         <v>188</v>
       </c>
       <c r="C49" t="s">
-        <v>577</v>
+        <v>555</v>
       </c>
       <c r="D49" t="s">
-        <v>578</v>
+        <v>556</v>
       </c>
       <c r="E49" t="s">
-        <v>579</v>
+        <v>557</v>
       </c>
       <c r="F49" t="s">
-        <v>580</v>
+        <v>558</v>
       </c>
       <c r="G49" t="s">
-        <v>581</v>
+        <v>559</v>
       </c>
       <c r="H49" t="s">
-        <v>582</v>
+        <v>984</v>
       </c>
       <c r="I49" t="s">
-        <v>583</v>
+        <v>560</v>
       </c>
       <c r="J49" t="s">
-        <v>584</v>
+        <v>561</v>
       </c>
       <c r="K49" t="s">
         <v>100</v>
@@ -5469,28 +5469,28 @@
         <v>191</v>
       </c>
       <c r="C50" t="s">
-        <v>585</v>
+        <v>562</v>
       </c>
       <c r="D50" t="s">
-        <v>586</v>
+        <v>563</v>
       </c>
       <c r="E50" t="s">
-        <v>587</v>
+        <v>564</v>
       </c>
       <c r="F50" t="s">
-        <v>588</v>
+        <v>565</v>
       </c>
       <c r="G50" t="s">
-        <v>589</v>
+        <v>566</v>
       </c>
       <c r="H50" t="s">
-        <v>590</v>
+        <v>985</v>
       </c>
       <c r="I50" t="s">
-        <v>591</v>
+        <v>567</v>
       </c>
       <c r="J50" t="s">
-        <v>592</v>
+        <v>568</v>
       </c>
       <c r="K50" t="s">
         <v>102</v>
@@ -5516,28 +5516,28 @@
         <v>194</v>
       </c>
       <c r="C51" t="s">
-        <v>593</v>
+        <v>569</v>
       </c>
       <c r="D51" t="s">
-        <v>594</v>
+        <v>570</v>
       </c>
       <c r="E51" t="s">
-        <v>595</v>
+        <v>571</v>
       </c>
       <c r="F51" t="s">
-        <v>596</v>
+        <v>572</v>
       </c>
       <c r="G51" t="s">
-        <v>597</v>
+        <v>573</v>
       </c>
       <c r="H51" t="s">
-        <v>598</v>
+        <v>986</v>
       </c>
       <c r="I51" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="J51" t="s">
-        <v>600</v>
+        <v>575</v>
       </c>
       <c r="K51" t="s">
         <v>104</v>
@@ -5563,28 +5563,28 @@
         <v>197</v>
       </c>
       <c r="C52" t="s">
-        <v>601</v>
+        <v>576</v>
       </c>
       <c r="D52" t="s">
-        <v>602</v>
+        <v>577</v>
       </c>
       <c r="E52" t="s">
-        <v>603</v>
+        <v>578</v>
       </c>
       <c r="F52" t="s">
-        <v>604</v>
+        <v>579</v>
       </c>
       <c r="G52" t="s">
-        <v>605</v>
+        <v>580</v>
       </c>
       <c r="H52" t="s">
-        <v>606</v>
+        <v>581</v>
       </c>
       <c r="I52" t="s">
-        <v>607</v>
+        <v>582</v>
       </c>
       <c r="J52" t="s">
-        <v>608</v>
+        <v>583</v>
       </c>
       <c r="K52" t="s">
         <v>106</v>
@@ -5610,28 +5610,28 @@
         <v>199</v>
       </c>
       <c r="C53" t="s">
-        <v>609</v>
+        <v>584</v>
       </c>
       <c r="D53" t="s">
-        <v>610</v>
+        <v>585</v>
       </c>
       <c r="E53" t="s">
-        <v>611</v>
+        <v>586</v>
       </c>
       <c r="F53" t="s">
-        <v>612</v>
+        <v>587</v>
       </c>
       <c r="G53" t="s">
-        <v>613</v>
+        <v>588</v>
       </c>
       <c r="H53" t="s">
-        <v>614</v>
+        <v>987</v>
       </c>
       <c r="I53" t="s">
-        <v>615</v>
+        <v>589</v>
       </c>
       <c r="J53" t="s">
-        <v>616</v>
+        <v>590</v>
       </c>
       <c r="K53" t="s">
         <v>109</v>
@@ -5657,28 +5657,28 @@
         <v>202</v>
       </c>
       <c r="C54" t="s">
-        <v>617</v>
+        <v>591</v>
       </c>
       <c r="D54" t="s">
-        <v>618</v>
+        <v>592</v>
       </c>
       <c r="E54" t="s">
-        <v>619</v>
+        <v>593</v>
       </c>
       <c r="F54" t="s">
-        <v>620</v>
+        <v>594</v>
       </c>
       <c r="G54" t="s">
-        <v>621</v>
+        <v>595</v>
       </c>
       <c r="H54" t="s">
-        <v>622</v>
+        <v>988</v>
       </c>
       <c r="I54" t="s">
-        <v>623</v>
+        <v>596</v>
       </c>
       <c r="J54" t="s">
-        <v>624</v>
+        <v>597</v>
       </c>
       <c r="K54" t="s">
         <v>111</v>
@@ -5704,28 +5704,28 @@
         <v>255</v>
       </c>
       <c r="C55" t="s">
-        <v>625</v>
+        <v>598</v>
       </c>
       <c r="D55" t="s">
-        <v>626</v>
+        <v>599</v>
       </c>
       <c r="E55" t="s">
-        <v>627</v>
+        <v>600</v>
       </c>
       <c r="F55" t="s">
-        <v>628</v>
+        <v>601</v>
       </c>
       <c r="G55" t="s">
-        <v>629</v>
+        <v>602</v>
       </c>
       <c r="H55" t="s">
-        <v>630</v>
+        <v>989</v>
       </c>
       <c r="I55" t="s">
-        <v>631</v>
+        <v>603</v>
       </c>
       <c r="J55" t="s">
-        <v>632</v>
+        <v>604</v>
       </c>
       <c r="K55" t="s">
         <v>97</v>
@@ -5751,28 +5751,28 @@
         <v>256</v>
       </c>
       <c r="C56" t="s">
-        <v>633</v>
+        <v>605</v>
       </c>
       <c r="D56" t="s">
-        <v>634</v>
+        <v>606</v>
       </c>
       <c r="E56" t="s">
-        <v>635</v>
+        <v>607</v>
       </c>
       <c r="F56" t="s">
-        <v>636</v>
+        <v>608</v>
       </c>
       <c r="G56" t="s">
-        <v>637</v>
+        <v>609</v>
       </c>
       <c r="H56" t="s">
-        <v>638</v>
+        <v>990</v>
       </c>
       <c r="I56" t="s">
-        <v>639</v>
+        <v>610</v>
       </c>
       <c r="J56" t="s">
-        <v>640</v>
+        <v>611</v>
       </c>
       <c r="K56" t="s">
         <v>114</v>
@@ -5798,28 +5798,28 @@
         <v>205</v>
       </c>
       <c r="C57" t="s">
-        <v>641</v>
+        <v>612</v>
       </c>
       <c r="D57" t="s">
-        <v>642</v>
+        <v>613</v>
       </c>
       <c r="E57" t="s">
-        <v>643</v>
+        <v>614</v>
       </c>
       <c r="F57" t="s">
-        <v>644</v>
+        <v>615</v>
       </c>
       <c r="G57" t="s">
-        <v>645</v>
+        <v>616</v>
       </c>
       <c r="H57" t="s">
-        <v>646</v>
+        <v>617</v>
       </c>
       <c r="I57" t="s">
-        <v>647</v>
+        <v>618</v>
       </c>
       <c r="J57" t="s">
-        <v>648</v>
+        <v>619</v>
       </c>
       <c r="K57" t="s">
         <v>14</v>
@@ -5845,28 +5845,28 @@
         <v>209</v>
       </c>
       <c r="C58" t="s">
-        <v>649</v>
+        <v>620</v>
       </c>
       <c r="D58" t="s">
-        <v>650</v>
+        <v>621</v>
       </c>
       <c r="E58" t="s">
-        <v>651</v>
+        <v>622</v>
       </c>
       <c r="F58" t="s">
-        <v>652</v>
+        <v>623</v>
       </c>
       <c r="G58" t="s">
-        <v>653</v>
+        <v>624</v>
       </c>
       <c r="H58" t="s">
-        <v>654</v>
+        <v>991</v>
       </c>
       <c r="I58" t="s">
-        <v>655</v>
+        <v>625</v>
       </c>
       <c r="J58" t="s">
-        <v>656</v>
+        <v>626</v>
       </c>
       <c r="K58" t="s">
         <v>16</v>
@@ -5892,28 +5892,28 @@
         <v>213</v>
       </c>
       <c r="C59" t="s">
-        <v>657</v>
+        <v>627</v>
       </c>
       <c r="D59" t="s">
-        <v>658</v>
+        <v>628</v>
       </c>
       <c r="E59" t="s">
-        <v>659</v>
+        <v>629</v>
       </c>
       <c r="F59" t="s">
-        <v>660</v>
+        <v>630</v>
       </c>
       <c r="G59" t="s">
-        <v>661</v>
+        <v>631</v>
       </c>
       <c r="H59" t="s">
-        <v>662</v>
+        <v>992</v>
       </c>
       <c r="I59" t="s">
-        <v>663</v>
+        <v>632</v>
       </c>
       <c r="J59" t="s">
-        <v>664</v>
+        <v>633</v>
       </c>
       <c r="K59" t="s">
         <v>18</v>
@@ -5939,28 +5939,28 @@
         <v>217</v>
       </c>
       <c r="C60" t="s">
-        <v>665</v>
+        <v>634</v>
       </c>
       <c r="D60" t="s">
-        <v>666</v>
+        <v>635</v>
       </c>
       <c r="E60" t="s">
-        <v>667</v>
+        <v>636</v>
       </c>
       <c r="F60" t="s">
-        <v>668</v>
+        <v>637</v>
       </c>
       <c r="G60" t="s">
-        <v>669</v>
+        <v>638</v>
       </c>
       <c r="H60" t="s">
-        <v>670</v>
+        <v>993</v>
       </c>
       <c r="I60" t="s">
-        <v>671</v>
+        <v>639</v>
       </c>
       <c r="J60" t="s">
-        <v>672</v>
+        <v>640</v>
       </c>
       <c r="K60" t="s">
         <v>20</v>
@@ -5986,28 +5986,28 @@
         <v>221</v>
       </c>
       <c r="C61" t="s">
-        <v>673</v>
+        <v>641</v>
       </c>
       <c r="D61" t="s">
-        <v>674</v>
+        <v>642</v>
       </c>
       <c r="E61" t="s">
-        <v>675</v>
+        <v>643</v>
       </c>
       <c r="F61" t="s">
-        <v>676</v>
+        <v>644</v>
       </c>
       <c r="G61" t="s">
-        <v>677</v>
+        <v>645</v>
       </c>
       <c r="H61" t="s">
-        <v>678</v>
+        <v>994</v>
       </c>
       <c r="I61" t="s">
-        <v>679</v>
+        <v>646</v>
       </c>
       <c r="J61" t="s">
-        <v>680</v>
+        <v>647</v>
       </c>
       <c r="K61" t="s">
         <v>23</v>
@@ -6033,28 +6033,28 @@
         <v>225</v>
       </c>
       <c r="C62" t="s">
-        <v>681</v>
+        <v>648</v>
       </c>
       <c r="D62" t="s">
-        <v>682</v>
+        <v>649</v>
       </c>
       <c r="E62" t="s">
-        <v>683</v>
+        <v>650</v>
       </c>
       <c r="F62" t="s">
-        <v>684</v>
+        <v>651</v>
       </c>
       <c r="G62" t="s">
-        <v>685</v>
+        <v>652</v>
       </c>
       <c r="H62" t="s">
-        <v>686</v>
+        <v>653</v>
       </c>
       <c r="I62" t="s">
-        <v>687</v>
+        <v>654</v>
       </c>
       <c r="J62" t="s">
-        <v>688</v>
+        <v>655</v>
       </c>
       <c r="K62" t="s">
         <v>25</v>
@@ -6080,28 +6080,28 @@
         <v>229</v>
       </c>
       <c r="C63" t="s">
-        <v>689</v>
+        <v>656</v>
       </c>
       <c r="D63" t="s">
-        <v>690</v>
+        <v>657</v>
       </c>
       <c r="E63" t="s">
-        <v>691</v>
+        <v>658</v>
       </c>
       <c r="F63" t="s">
-        <v>692</v>
+        <v>659</v>
       </c>
       <c r="G63" t="s">
-        <v>693</v>
+        <v>660</v>
       </c>
       <c r="H63" t="s">
-        <v>694</v>
+        <v>995</v>
       </c>
       <c r="I63" t="s">
-        <v>695</v>
+        <v>661</v>
       </c>
       <c r="J63" t="s">
-        <v>696</v>
+        <v>662</v>
       </c>
       <c r="K63" t="s">
         <v>27</v>
@@ -6127,28 +6127,28 @@
         <v>233</v>
       </c>
       <c r="C64" t="s">
-        <v>697</v>
+        <v>663</v>
       </c>
       <c r="D64" t="s">
-        <v>698</v>
+        <v>664</v>
       </c>
       <c r="E64" t="s">
-        <v>699</v>
+        <v>665</v>
       </c>
       <c r="F64" t="s">
-        <v>700</v>
+        <v>666</v>
       </c>
       <c r="G64" t="s">
-        <v>701</v>
+        <v>667</v>
       </c>
       <c r="H64" t="s">
-        <v>702</v>
+        <v>996</v>
       </c>
       <c r="I64" t="s">
-        <v>703</v>
+        <v>668</v>
       </c>
       <c r="J64" t="s">
-        <v>704</v>
+        <v>669</v>
       </c>
       <c r="K64" t="s">
         <v>29</v>
@@ -6174,28 +6174,28 @@
         <v>237</v>
       </c>
       <c r="C65" t="s">
-        <v>705</v>
+        <v>670</v>
       </c>
       <c r="D65" t="s">
-        <v>706</v>
+        <v>671</v>
       </c>
       <c r="E65" t="s">
-        <v>707</v>
+        <v>672</v>
       </c>
       <c r="F65" t="s">
-        <v>708</v>
+        <v>673</v>
       </c>
       <c r="G65" t="s">
-        <v>709</v>
+        <v>674</v>
       </c>
       <c r="H65" t="s">
-        <v>710</v>
+        <v>997</v>
       </c>
       <c r="I65" t="s">
-        <v>711</v>
+        <v>675</v>
       </c>
       <c r="J65" t="s">
-        <v>712</v>
+        <v>676</v>
       </c>
       <c r="K65" t="s">
         <v>32</v>
@@ -6221,28 +6221,28 @@
         <v>241</v>
       </c>
       <c r="C66" t="s">
-        <v>713</v>
+        <v>677</v>
       </c>
       <c r="D66" t="s">
-        <v>714</v>
+        <v>678</v>
       </c>
       <c r="E66" t="s">
-        <v>715</v>
+        <v>679</v>
       </c>
       <c r="F66" t="s">
-        <v>716</v>
+        <v>680</v>
       </c>
       <c r="G66" t="s">
-        <v>717</v>
+        <v>681</v>
       </c>
       <c r="H66" t="s">
-        <v>718</v>
+        <v>998</v>
       </c>
       <c r="I66" t="s">
-        <v>719</v>
+        <v>682</v>
       </c>
       <c r="J66" t="s">
-        <v>720</v>
+        <v>683</v>
       </c>
       <c r="K66" t="s">
         <v>34</v>
@@ -6268,28 +6268,28 @@
         <v>245</v>
       </c>
       <c r="C67" t="s">
-        <v>721</v>
+        <v>684</v>
       </c>
       <c r="D67" t="s">
-        <v>722</v>
+        <v>685</v>
       </c>
       <c r="E67" t="s">
-        <v>723</v>
+        <v>686</v>
       </c>
       <c r="F67" t="s">
-        <v>724</v>
+        <v>687</v>
       </c>
       <c r="G67" t="s">
-        <v>725</v>
+        <v>688</v>
       </c>
       <c r="H67" t="s">
-        <v>726</v>
+        <v>689</v>
       </c>
       <c r="I67" t="s">
-        <v>727</v>
+        <v>690</v>
       </c>
       <c r="J67" t="s">
-        <v>728</v>
+        <v>691</v>
       </c>
       <c r="K67" t="s">
         <v>36</v>
@@ -6315,28 +6315,28 @@
         <v>249</v>
       </c>
       <c r="C68" t="s">
-        <v>729</v>
+        <v>692</v>
       </c>
       <c r="D68" t="s">
-        <v>730</v>
+        <v>693</v>
       </c>
       <c r="E68" t="s">
-        <v>731</v>
+        <v>694</v>
       </c>
       <c r="F68" t="s">
-        <v>732</v>
+        <v>695</v>
       </c>
       <c r="G68" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H68" t="s">
-        <v>733</v>
+        <v>999</v>
       </c>
       <c r="I68" t="s">
-        <v>734</v>
+        <v>696</v>
       </c>
       <c r="J68" t="s">
-        <v>735</v>
+        <v>697</v>
       </c>
       <c r="K68" t="s">
         <v>38</v>
@@ -6362,28 +6362,28 @@
         <v>206</v>
       </c>
       <c r="C69" t="s">
-        <v>736</v>
+        <v>698</v>
       </c>
       <c r="D69" t="s">
-        <v>737</v>
+        <v>699</v>
       </c>
       <c r="E69" t="s">
-        <v>738</v>
+        <v>700</v>
       </c>
       <c r="F69" t="s">
-        <v>739</v>
+        <v>701</v>
       </c>
       <c r="G69" t="s">
-        <v>740</v>
+        <v>702</v>
       </c>
       <c r="H69" t="s">
-        <v>741</v>
+        <v>1000</v>
       </c>
       <c r="I69" t="s">
-        <v>742</v>
+        <v>703</v>
       </c>
       <c r="J69" t="s">
-        <v>743</v>
+        <v>704</v>
       </c>
       <c r="K69" t="s">
         <v>41</v>
@@ -6409,28 +6409,28 @@
         <v>210</v>
       </c>
       <c r="C70" t="s">
-        <v>744</v>
+        <v>705</v>
       </c>
       <c r="D70" t="s">
-        <v>745</v>
+        <v>706</v>
       </c>
       <c r="E70" t="s">
-        <v>746</v>
+        <v>707</v>
       </c>
       <c r="F70" t="s">
-        <v>747</v>
+        <v>708</v>
       </c>
       <c r="G70" t="s">
-        <v>748</v>
+        <v>709</v>
       </c>
       <c r="H70" t="s">
-        <v>749</v>
+        <v>1001</v>
       </c>
       <c r="I70" t="s">
-        <v>750</v>
+        <v>710</v>
       </c>
       <c r="J70" t="s">
-        <v>751</v>
+        <v>711</v>
       </c>
       <c r="K70" t="s">
         <v>43</v>
@@ -6456,28 +6456,28 @@
         <v>214</v>
       </c>
       <c r="C71" t="s">
-        <v>752</v>
+        <v>712</v>
       </c>
       <c r="D71" t="s">
-        <v>753</v>
+        <v>713</v>
       </c>
       <c r="E71" t="s">
-        <v>754</v>
+        <v>714</v>
       </c>
       <c r="F71" t="s">
-        <v>755</v>
+        <v>715</v>
       </c>
       <c r="G71" t="s">
-        <v>756</v>
+        <v>716</v>
       </c>
       <c r="H71" t="s">
-        <v>757</v>
+        <v>717</v>
       </c>
       <c r="I71" t="s">
-        <v>758</v>
+        <v>718</v>
       </c>
       <c r="J71" t="s">
-        <v>759</v>
+        <v>719</v>
       </c>
       <c r="K71" t="s">
         <v>45</v>
@@ -6503,28 +6503,28 @@
         <v>218</v>
       </c>
       <c r="C72" t="s">
-        <v>760</v>
+        <v>720</v>
       </c>
       <c r="D72" t="s">
-        <v>761</v>
+        <v>721</v>
       </c>
       <c r="E72" t="s">
-        <v>762</v>
+        <v>722</v>
       </c>
       <c r="F72" t="s">
-        <v>763</v>
+        <v>723</v>
       </c>
       <c r="G72" t="s">
-        <v>764</v>
+        <v>724</v>
       </c>
       <c r="H72" t="s">
-        <v>765</v>
+        <v>725</v>
       </c>
       <c r="I72" t="s">
-        <v>766</v>
+        <v>726</v>
       </c>
       <c r="J72" t="s">
-        <v>767</v>
+        <v>727</v>
       </c>
       <c r="K72" t="s">
         <v>47</v>
@@ -6550,28 +6550,28 @@
         <v>222</v>
       </c>
       <c r="C73" t="s">
-        <v>768</v>
+        <v>728</v>
       </c>
       <c r="D73" t="s">
-        <v>769</v>
+        <v>729</v>
       </c>
       <c r="E73" t="s">
-        <v>770</v>
+        <v>730</v>
       </c>
       <c r="F73" t="s">
-        <v>771</v>
+        <v>731</v>
       </c>
       <c r="G73" t="s">
-        <v>772</v>
+        <v>732</v>
       </c>
       <c r="H73" t="s">
-        <v>773</v>
+        <v>733</v>
       </c>
       <c r="I73" t="s">
-        <v>774</v>
+        <v>734</v>
       </c>
       <c r="J73" t="s">
-        <v>775</v>
+        <v>735</v>
       </c>
       <c r="K73" t="s">
         <v>50</v>
@@ -6597,28 +6597,28 @@
         <v>226</v>
       </c>
       <c r="C74" t="s">
-        <v>776</v>
+        <v>736</v>
       </c>
       <c r="D74" t="s">
-        <v>777</v>
+        <v>737</v>
       </c>
       <c r="E74" t="s">
-        <v>778</v>
+        <v>738</v>
       </c>
       <c r="F74" t="s">
-        <v>779</v>
+        <v>739</v>
       </c>
       <c r="G74" t="s">
-        <v>780</v>
+        <v>740</v>
       </c>
       <c r="H74" t="s">
-        <v>781</v>
+        <v>741</v>
       </c>
       <c r="I74" t="s">
-        <v>782</v>
+        <v>742</v>
       </c>
       <c r="J74" t="s">
-        <v>783</v>
+        <v>743</v>
       </c>
       <c r="K74" t="s">
         <v>52</v>
@@ -6644,28 +6644,28 @@
         <v>230</v>
       </c>
       <c r="C75" t="s">
-        <v>784</v>
+        <v>744</v>
       </c>
       <c r="D75" t="s">
-        <v>785</v>
+        <v>745</v>
       </c>
       <c r="E75" t="s">
-        <v>786</v>
+        <v>746</v>
       </c>
       <c r="F75" t="s">
-        <v>787</v>
+        <v>747</v>
       </c>
       <c r="G75" t="s">
-        <v>788</v>
+        <v>748</v>
       </c>
       <c r="H75" t="s">
-        <v>789</v>
+        <v>1002</v>
       </c>
       <c r="I75" t="s">
-        <v>790</v>
+        <v>749</v>
       </c>
       <c r="J75" t="s">
-        <v>791</v>
+        <v>750</v>
       </c>
       <c r="K75" t="s">
         <v>54</v>
@@ -6691,28 +6691,28 @@
         <v>234</v>
       </c>
       <c r="C76" t="s">
-        <v>792</v>
+        <v>751</v>
       </c>
       <c r="D76" t="s">
-        <v>793</v>
+        <v>752</v>
       </c>
       <c r="E76" t="s">
-        <v>794</v>
+        <v>753</v>
       </c>
       <c r="F76" t="s">
-        <v>795</v>
+        <v>754</v>
       </c>
       <c r="G76" t="s">
-        <v>796</v>
+        <v>755</v>
       </c>
       <c r="H76" t="s">
-        <v>797</v>
+        <v>1003</v>
       </c>
       <c r="I76" t="s">
-        <v>798</v>
+        <v>756</v>
       </c>
       <c r="J76" t="s">
-        <v>799</v>
+        <v>757</v>
       </c>
       <c r="K76" t="s">
         <v>16</v>
@@ -6738,28 +6738,28 @@
         <v>238</v>
       </c>
       <c r="C77" t="s">
-        <v>800</v>
+        <v>758</v>
       </c>
       <c r="D77" t="s">
-        <v>801</v>
+        <v>759</v>
       </c>
       <c r="E77" t="s">
-        <v>802</v>
+        <v>760</v>
       </c>
       <c r="F77" t="s">
-        <v>803</v>
+        <v>761</v>
       </c>
       <c r="G77" t="s">
-        <v>804</v>
+        <v>762</v>
       </c>
       <c r="H77" t="s">
-        <v>805</v>
+        <v>1004</v>
       </c>
       <c r="I77" t="s">
-        <v>806</v>
+        <v>763</v>
       </c>
       <c r="J77" t="s">
-        <v>807</v>
+        <v>764</v>
       </c>
       <c r="K77" t="s">
         <v>58</v>
@@ -6785,28 +6785,28 @@
         <v>242</v>
       </c>
       <c r="C78" t="s">
-        <v>808</v>
+        <v>765</v>
       </c>
       <c r="D78" t="s">
-        <v>809</v>
+        <v>766</v>
       </c>
       <c r="E78" t="s">
-        <v>810</v>
+        <v>767</v>
       </c>
       <c r="F78" t="s">
-        <v>811</v>
+        <v>768</v>
       </c>
       <c r="G78" t="s">
-        <v>812</v>
+        <v>769</v>
       </c>
       <c r="H78" t="s">
-        <v>813</v>
+        <v>770</v>
       </c>
       <c r="I78" t="s">
-        <v>814</v>
+        <v>771</v>
       </c>
       <c r="J78" t="s">
-        <v>815</v>
+        <v>772</v>
       </c>
       <c r="K78" t="s">
         <v>60</v>
@@ -6832,28 +6832,28 @@
         <v>246</v>
       </c>
       <c r="C79" t="s">
-        <v>816</v>
+        <v>773</v>
       </c>
       <c r="D79" t="s">
-        <v>817</v>
+        <v>774</v>
       </c>
       <c r="E79" t="s">
-        <v>818</v>
+        <v>775</v>
       </c>
       <c r="F79" t="s">
-        <v>819</v>
+        <v>776</v>
       </c>
       <c r="G79" t="s">
-        <v>820</v>
+        <v>777</v>
       </c>
       <c r="H79" t="s">
-        <v>821</v>
+        <v>778</v>
       </c>
       <c r="I79" t="s">
-        <v>822</v>
+        <v>779</v>
       </c>
       <c r="J79" t="s">
-        <v>823</v>
+        <v>780</v>
       </c>
       <c r="K79" t="s">
         <v>62</v>
@@ -6879,28 +6879,28 @@
         <v>250</v>
       </c>
       <c r="C80" t="s">
-        <v>824</v>
+        <v>781</v>
       </c>
       <c r="D80" t="s">
-        <v>825</v>
+        <v>782</v>
       </c>
       <c r="E80" t="s">
-        <v>826</v>
+        <v>783</v>
       </c>
       <c r="F80" t="s">
-        <v>827</v>
+        <v>784</v>
       </c>
       <c r="G80" t="s">
-        <v>828</v>
+        <v>785</v>
       </c>
       <c r="H80" t="s">
-        <v>829</v>
+        <v>1005</v>
       </c>
       <c r="I80" t="s">
-        <v>830</v>
+        <v>786</v>
       </c>
       <c r="J80" t="s">
-        <v>831</v>
+        <v>787</v>
       </c>
       <c r="K80" t="s">
         <v>64</v>
@@ -6926,28 +6926,28 @@
         <v>207</v>
       </c>
       <c r="C81" t="s">
-        <v>832</v>
+        <v>788</v>
       </c>
       <c r="D81" t="s">
-        <v>833</v>
+        <v>789</v>
       </c>
       <c r="E81" t="s">
-        <v>834</v>
+        <v>790</v>
       </c>
       <c r="F81" t="s">
-        <v>835</v>
+        <v>791</v>
       </c>
       <c r="G81" t="s">
-        <v>836</v>
+        <v>792</v>
       </c>
       <c r="H81" t="s">
-        <v>837</v>
+        <v>793</v>
       </c>
       <c r="I81" t="s">
-        <v>838</v>
+        <v>794</v>
       </c>
       <c r="J81" t="s">
-        <v>839</v>
+        <v>795</v>
       </c>
       <c r="K81" t="s">
         <v>67</v>
@@ -6973,28 +6973,28 @@
         <v>211</v>
       </c>
       <c r="C82" t="s">
-        <v>840</v>
+        <v>796</v>
       </c>
       <c r="D82" t="s">
-        <v>841</v>
+        <v>797</v>
       </c>
       <c r="E82" t="s">
-        <v>842</v>
+        <v>798</v>
       </c>
       <c r="F82" t="s">
-        <v>843</v>
+        <v>799</v>
       </c>
       <c r="G82" t="s">
-        <v>844</v>
+        <v>800</v>
       </c>
       <c r="H82" t="s">
-        <v>845</v>
+        <v>1006</v>
       </c>
       <c r="I82" t="s">
-        <v>846</v>
+        <v>801</v>
       </c>
       <c r="J82" t="s">
-        <v>847</v>
+        <v>802</v>
       </c>
       <c r="K82" t="s">
         <v>69</v>
@@ -7020,28 +7020,28 @@
         <v>215</v>
       </c>
       <c r="C83" t="s">
-        <v>848</v>
+        <v>803</v>
       </c>
       <c r="D83" t="s">
-        <v>849</v>
+        <v>804</v>
       </c>
       <c r="E83" t="s">
-        <v>850</v>
+        <v>805</v>
       </c>
       <c r="F83" t="s">
-        <v>851</v>
+        <v>806</v>
       </c>
       <c r="G83" t="s">
-        <v>852</v>
+        <v>807</v>
       </c>
       <c r="H83" t="s">
-        <v>853</v>
+        <v>1007</v>
       </c>
       <c r="I83" t="s">
-        <v>854</v>
+        <v>808</v>
       </c>
       <c r="J83" t="s">
-        <v>855</v>
+        <v>809</v>
       </c>
       <c r="K83" t="s">
         <v>71</v>
@@ -7067,28 +7067,28 @@
         <v>219</v>
       </c>
       <c r="C84" t="s">
-        <v>856</v>
+        <v>810</v>
       </c>
       <c r="D84" t="s">
-        <v>857</v>
+        <v>811</v>
       </c>
       <c r="E84" t="s">
-        <v>858</v>
+        <v>812</v>
       </c>
       <c r="F84" t="s">
-        <v>859</v>
+        <v>813</v>
       </c>
       <c r="G84" t="s">
-        <v>860</v>
+        <v>814</v>
       </c>
       <c r="H84" t="s">
-        <v>861</v>
+        <v>1008</v>
       </c>
       <c r="I84" t="s">
-        <v>862</v>
+        <v>815</v>
       </c>
       <c r="J84" t="s">
-        <v>863</v>
+        <v>816</v>
       </c>
       <c r="K84" t="s">
         <v>29</v>
@@ -7114,28 +7114,28 @@
         <v>223</v>
       </c>
       <c r="C85" t="s">
-        <v>864</v>
+        <v>817</v>
       </c>
       <c r="D85" t="s">
-        <v>865</v>
+        <v>818</v>
       </c>
       <c r="E85" t="s">
-        <v>866</v>
+        <v>819</v>
       </c>
       <c r="F85" t="s">
-        <v>867</v>
+        <v>820</v>
       </c>
       <c r="G85" t="s">
-        <v>868</v>
+        <v>821</v>
       </c>
       <c r="H85" t="s">
-        <v>869</v>
+        <v>1009</v>
       </c>
       <c r="I85" t="s">
-        <v>870</v>
+        <v>822</v>
       </c>
       <c r="J85" t="s">
-        <v>871</v>
+        <v>823</v>
       </c>
       <c r="K85" t="s">
         <v>75</v>
@@ -7161,28 +7161,28 @@
         <v>227</v>
       </c>
       <c r="C86" t="s">
-        <v>872</v>
+        <v>824</v>
       </c>
       <c r="D86" t="s">
-        <v>873</v>
+        <v>825</v>
       </c>
       <c r="E86" t="s">
-        <v>874</v>
+        <v>826</v>
       </c>
       <c r="F86" t="s">
-        <v>875</v>
+        <v>827</v>
       </c>
       <c r="G86" t="s">
-        <v>876</v>
+        <v>828</v>
       </c>
       <c r="H86" t="s">
-        <v>877</v>
+        <v>829</v>
       </c>
       <c r="I86" t="s">
-        <v>878</v>
+        <v>830</v>
       </c>
       <c r="J86" t="s">
-        <v>879</v>
+        <v>831</v>
       </c>
       <c r="K86" t="s">
         <v>77</v>
@@ -7208,28 +7208,28 @@
         <v>231</v>
       </c>
       <c r="C87" t="s">
-        <v>880</v>
+        <v>832</v>
       </c>
       <c r="D87" t="s">
-        <v>881</v>
+        <v>833</v>
       </c>
       <c r="E87" t="s">
-        <v>882</v>
+        <v>834</v>
       </c>
       <c r="F87" t="s">
-        <v>883</v>
+        <v>835</v>
       </c>
       <c r="G87" t="s">
-        <v>884</v>
+        <v>836</v>
       </c>
       <c r="H87" t="s">
-        <v>885</v>
+        <v>1010</v>
       </c>
       <c r="I87" t="s">
-        <v>886</v>
+        <v>837</v>
       </c>
       <c r="J87" t="s">
-        <v>887</v>
+        <v>838</v>
       </c>
       <c r="K87" t="s">
         <v>79</v>
@@ -7255,28 +7255,28 @@
         <v>235</v>
       </c>
       <c r="C88" t="s">
-        <v>888</v>
+        <v>839</v>
       </c>
       <c r="D88" t="s">
-        <v>889</v>
+        <v>840</v>
       </c>
       <c r="E88" t="s">
-        <v>890</v>
+        <v>841</v>
       </c>
       <c r="F88" t="s">
-        <v>891</v>
+        <v>842</v>
       </c>
       <c r="G88" t="s">
-        <v>892</v>
+        <v>843</v>
       </c>
       <c r="H88" t="s">
-        <v>893</v>
+        <v>844</v>
       </c>
       <c r="I88" t="s">
-        <v>894</v>
+        <v>845</v>
       </c>
       <c r="J88" t="s">
-        <v>895</v>
+        <v>846</v>
       </c>
       <c r="K88" t="s">
         <v>81</v>
@@ -7302,28 +7302,28 @@
         <v>239</v>
       </c>
       <c r="C89" t="s">
-        <v>896</v>
+        <v>847</v>
       </c>
       <c r="D89" t="s">
-        <v>897</v>
+        <v>848</v>
       </c>
       <c r="E89" t="s">
-        <v>898</v>
+        <v>849</v>
       </c>
       <c r="F89" t="s">
-        <v>899</v>
+        <v>850</v>
       </c>
       <c r="G89" t="s">
-        <v>900</v>
+        <v>851</v>
       </c>
       <c r="H89" t="s">
-        <v>901</v>
+        <v>1011</v>
       </c>
       <c r="I89" t="s">
-        <v>902</v>
+        <v>852</v>
       </c>
       <c r="J89" t="s">
-        <v>903</v>
+        <v>853</v>
       </c>
       <c r="K89" t="s">
         <v>84</v>
@@ -7349,28 +7349,28 @@
         <v>243</v>
       </c>
       <c r="C90" t="s">
-        <v>904</v>
+        <v>854</v>
       </c>
       <c r="D90" t="s">
-        <v>905</v>
+        <v>855</v>
       </c>
       <c r="E90" t="s">
-        <v>906</v>
+        <v>856</v>
       </c>
       <c r="F90" t="s">
-        <v>907</v>
+        <v>857</v>
       </c>
       <c r="G90" t="s">
-        <v>908</v>
+        <v>858</v>
       </c>
       <c r="H90" t="s">
-        <v>909</v>
+        <v>1012</v>
       </c>
       <c r="I90" t="s">
-        <v>910</v>
+        <v>859</v>
       </c>
       <c r="J90" t="s">
-        <v>911</v>
+        <v>860</v>
       </c>
       <c r="K90" t="s">
         <v>86</v>
@@ -7396,28 +7396,28 @@
         <v>247</v>
       </c>
       <c r="C91" t="s">
-        <v>912</v>
+        <v>861</v>
       </c>
       <c r="D91" t="s">
-        <v>913</v>
+        <v>862</v>
       </c>
       <c r="E91" t="s">
-        <v>914</v>
+        <v>863</v>
       </c>
       <c r="F91" t="s">
-        <v>915</v>
+        <v>864</v>
       </c>
       <c r="G91" t="s">
-        <v>916</v>
+        <v>865</v>
       </c>
       <c r="H91" t="s">
-        <v>917</v>
+        <v>866</v>
       </c>
       <c r="I91" t="s">
-        <v>918</v>
+        <v>867</v>
       </c>
       <c r="J91" t="s">
-        <v>919</v>
+        <v>868</v>
       </c>
       <c r="K91" t="s">
         <v>88</v>
@@ -7443,28 +7443,28 @@
         <v>251</v>
       </c>
       <c r="C92" t="s">
-        <v>920</v>
+        <v>869</v>
       </c>
       <c r="D92" t="s">
-        <v>921</v>
+        <v>870</v>
       </c>
       <c r="E92" t="s">
-        <v>922</v>
+        <v>871</v>
       </c>
       <c r="F92" t="s">
-        <v>923</v>
+        <v>872</v>
       </c>
       <c r="G92" t="s">
-        <v>924</v>
+        <v>873</v>
       </c>
       <c r="H92" t="s">
-        <v>925</v>
+        <v>1013</v>
       </c>
       <c r="I92" t="s">
-        <v>926</v>
+        <v>874</v>
       </c>
       <c r="J92" t="s">
-        <v>927</v>
+        <v>875</v>
       </c>
       <c r="K92" t="s">
         <v>81</v>
@@ -7490,28 +7490,28 @@
         <v>208</v>
       </c>
       <c r="C93" t="s">
-        <v>928</v>
+        <v>876</v>
       </c>
       <c r="D93" t="s">
-        <v>929</v>
+        <v>877</v>
       </c>
       <c r="E93" t="s">
-        <v>930</v>
+        <v>878</v>
       </c>
       <c r="F93" t="s">
-        <v>906</v>
+        <v>856</v>
       </c>
       <c r="G93" t="s">
-        <v>931</v>
+        <v>879</v>
       </c>
       <c r="H93" t="s">
-        <v>932</v>
+        <v>1014</v>
       </c>
       <c r="I93" t="s">
-        <v>933</v>
+        <v>880</v>
       </c>
       <c r="J93" t="s">
-        <v>934</v>
+        <v>881</v>
       </c>
       <c r="K93" t="s">
         <v>92</v>
@@ -7537,28 +7537,28 @@
         <v>212</v>
       </c>
       <c r="C94" t="s">
-        <v>935</v>
+        <v>882</v>
       </c>
       <c r="D94" t="s">
-        <v>936</v>
+        <v>883</v>
       </c>
       <c r="E94" t="s">
-        <v>937</v>
+        <v>884</v>
       </c>
       <c r="F94" t="s">
-        <v>938</v>
+        <v>885</v>
       </c>
       <c r="G94" t="s">
-        <v>939</v>
+        <v>886</v>
       </c>
       <c r="H94" t="s">
-        <v>940</v>
+        <v>887</v>
       </c>
       <c r="I94" t="s">
-        <v>941</v>
+        <v>888</v>
       </c>
       <c r="J94" t="s">
-        <v>942</v>
+        <v>889</v>
       </c>
       <c r="K94" t="s">
         <v>94</v>
@@ -7584,28 +7584,28 @@
         <v>216</v>
       </c>
       <c r="C95" t="s">
-        <v>943</v>
+        <v>890</v>
       </c>
       <c r="D95" t="s">
-        <v>944</v>
+        <v>891</v>
       </c>
       <c r="E95" t="s">
-        <v>945</v>
+        <v>892</v>
       </c>
       <c r="F95" t="s">
-        <v>946</v>
+        <v>893</v>
       </c>
       <c r="G95" t="s">
-        <v>947</v>
+        <v>894</v>
       </c>
       <c r="H95" t="s">
-        <v>948</v>
+        <v>1015</v>
       </c>
       <c r="I95" t="s">
-        <v>949</v>
+        <v>895</v>
       </c>
       <c r="J95" t="s">
-        <v>950</v>
+        <v>896</v>
       </c>
       <c r="K95" t="s">
         <v>47</v>
@@ -7631,28 +7631,28 @@
         <v>220</v>
       </c>
       <c r="C96" t="s">
-        <v>951</v>
+        <v>897</v>
       </c>
       <c r="D96" t="s">
-        <v>952</v>
+        <v>898</v>
       </c>
       <c r="E96" t="s">
-        <v>953</v>
+        <v>899</v>
       </c>
       <c r="F96" t="s">
-        <v>954</v>
+        <v>900</v>
       </c>
       <c r="G96" t="s">
-        <v>955</v>
+        <v>901</v>
       </c>
       <c r="H96" t="s">
-        <v>956</v>
+        <v>902</v>
       </c>
       <c r="I96" t="s">
-        <v>957</v>
+        <v>903</v>
       </c>
       <c r="J96" t="s">
-        <v>958</v>
+        <v>904</v>
       </c>
       <c r="K96" t="s">
         <v>97</v>
@@ -7678,28 +7678,28 @@
         <v>224</v>
       </c>
       <c r="C97" t="s">
-        <v>959</v>
+        <v>905</v>
       </c>
       <c r="D97" t="s">
-        <v>960</v>
+        <v>906</v>
       </c>
       <c r="E97" t="s">
-        <v>961</v>
+        <v>907</v>
       </c>
       <c r="F97" t="s">
-        <v>962</v>
+        <v>908</v>
       </c>
       <c r="G97" t="s">
-        <v>963</v>
+        <v>909</v>
       </c>
       <c r="H97" t="s">
-        <v>964</v>
+        <v>1016</v>
       </c>
       <c r="I97" t="s">
-        <v>965</v>
+        <v>910</v>
       </c>
       <c r="J97" t="s">
-        <v>966</v>
+        <v>911</v>
       </c>
       <c r="K97" t="s">
         <v>100</v>
@@ -7725,28 +7725,28 @@
         <v>228</v>
       </c>
       <c r="C98" t="s">
-        <v>967</v>
+        <v>912</v>
       </c>
       <c r="D98" t="s">
-        <v>968</v>
+        <v>913</v>
       </c>
       <c r="E98" t="s">
-        <v>969</v>
+        <v>914</v>
       </c>
       <c r="F98" t="s">
-        <v>970</v>
+        <v>915</v>
       </c>
       <c r="G98" t="s">
-        <v>971</v>
+        <v>916</v>
       </c>
       <c r="H98" t="s">
-        <v>972</v>
+        <v>917</v>
       </c>
       <c r="I98" t="s">
-        <v>973</v>
+        <v>918</v>
       </c>
       <c r="J98" t="s">
-        <v>974</v>
+        <v>919</v>
       </c>
       <c r="K98" t="s">
         <v>102</v>
@@ -7772,28 +7772,28 @@
         <v>232</v>
       </c>
       <c r="C99" t="s">
-        <v>975</v>
+        <v>920</v>
       </c>
       <c r="D99" t="s">
-        <v>976</v>
+        <v>921</v>
       </c>
       <c r="E99" t="s">
-        <v>977</v>
+        <v>922</v>
       </c>
       <c r="F99" t="s">
-        <v>978</v>
+        <v>923</v>
       </c>
       <c r="G99" t="s">
-        <v>979</v>
+        <v>924</v>
       </c>
       <c r="H99" t="s">
-        <v>980</v>
+        <v>1017</v>
       </c>
       <c r="I99" t="s">
-        <v>981</v>
+        <v>925</v>
       </c>
       <c r="J99" t="s">
-        <v>982</v>
+        <v>926</v>
       </c>
       <c r="K99" t="s">
         <v>104</v>
@@ -7819,28 +7819,28 @@
         <v>236</v>
       </c>
       <c r="C100" t="s">
-        <v>983</v>
+        <v>927</v>
       </c>
       <c r="D100" t="s">
-        <v>984</v>
+        <v>928</v>
       </c>
       <c r="E100" t="s">
-        <v>985</v>
+        <v>929</v>
       </c>
       <c r="F100" t="s">
-        <v>986</v>
+        <v>930</v>
       </c>
       <c r="G100" t="s">
-        <v>987</v>
+        <v>931</v>
       </c>
       <c r="H100" t="s">
-        <v>988</v>
+        <v>1018</v>
       </c>
       <c r="I100" t="s">
-        <v>989</v>
+        <v>932</v>
       </c>
       <c r="J100" t="s">
-        <v>990</v>
+        <v>933</v>
       </c>
       <c r="K100" t="s">
         <v>106</v>
@@ -7866,28 +7866,28 @@
         <v>240</v>
       </c>
       <c r="C101" t="s">
-        <v>991</v>
+        <v>934</v>
       </c>
       <c r="D101" t="s">
-        <v>992</v>
+        <v>935</v>
       </c>
       <c r="E101" t="s">
-        <v>993</v>
+        <v>936</v>
       </c>
       <c r="F101" t="s">
-        <v>994</v>
+        <v>937</v>
       </c>
       <c r="G101" t="s">
-        <v>725</v>
+        <v>688</v>
       </c>
       <c r="H101" t="s">
-        <v>995</v>
+        <v>938</v>
       </c>
       <c r="I101" t="s">
-        <v>996</v>
+        <v>939</v>
       </c>
       <c r="J101" t="s">
-        <v>997</v>
+        <v>940</v>
       </c>
       <c r="K101" t="s">
         <v>109</v>
@@ -7913,28 +7913,28 @@
         <v>244</v>
       </c>
       <c r="C102" t="s">
-        <v>998</v>
+        <v>941</v>
       </c>
       <c r="D102" t="s">
-        <v>999</v>
+        <v>942</v>
       </c>
       <c r="E102" t="s">
-        <v>1000</v>
+        <v>943</v>
       </c>
       <c r="F102" t="s">
-        <v>1001</v>
+        <v>944</v>
       </c>
       <c r="G102" t="s">
-        <v>1002</v>
+        <v>945</v>
       </c>
       <c r="H102" t="s">
-        <v>1003</v>
+        <v>1019</v>
       </c>
       <c r="I102" t="s">
-        <v>1004</v>
+        <v>946</v>
       </c>
       <c r="J102" t="s">
-        <v>1005</v>
+        <v>947</v>
       </c>
       <c r="K102" t="s">
         <v>111</v>
@@ -7960,28 +7960,28 @@
         <v>248</v>
       </c>
       <c r="C103" t="s">
-        <v>1006</v>
+        <v>948</v>
       </c>
       <c r="D103" t="s">
-        <v>1007</v>
+        <v>949</v>
       </c>
       <c r="E103" t="s">
-        <v>1008</v>
+        <v>950</v>
       </c>
       <c r="F103" t="s">
-        <v>1009</v>
+        <v>951</v>
       </c>
       <c r="G103" t="s">
-        <v>1010</v>
+        <v>952</v>
       </c>
       <c r="H103" t="s">
-        <v>1011</v>
+        <v>1020</v>
       </c>
       <c r="I103" t="s">
-        <v>1012</v>
+        <v>953</v>
       </c>
       <c r="J103" t="s">
-        <v>1013</v>
+        <v>954</v>
       </c>
       <c r="K103" t="s">
         <v>97</v>
@@ -8007,28 +8007,28 @@
         <v>252</v>
       </c>
       <c r="C104" t="s">
-        <v>1014</v>
+        <v>955</v>
       </c>
       <c r="D104" t="s">
-        <v>1015</v>
+        <v>956</v>
       </c>
       <c r="E104" t="s">
-        <v>1016</v>
+        <v>957</v>
       </c>
       <c r="F104" t="s">
-        <v>1017</v>
+        <v>958</v>
       </c>
       <c r="G104" t="s">
-        <v>1018</v>
+        <v>959</v>
       </c>
       <c r="H104" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="I104" t="s">
-        <v>1020</v>
+        <v>960</v>
       </c>
       <c r="J104" t="s">
-        <v>1021</v>
+        <v>961</v>
       </c>
       <c r="K104" t="s">
         <v>114</v>

</xml_diff>